<commit_message>
2nd commit tables arranged
</commit_message>
<xml_diff>
--- a/view-attendance/Attendance.xlsx
+++ b/view-attendance/Attendance.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://capgemini-my.sharepoint.com/personal/arth-shishir_sindekar_capgemini_com/Documents/Desktop/WebApp/view-attendance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="11_ECCF65358CB93E6120C31A6A40FD0CB4437A6517" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41A6C202-9408-484B-B590-168A4DFB56A8}"/>
+  <xr:revisionPtr revIDLastSave="101" documentId="11_ECCF65358CB93E6120C31A6A40FD0CB4437A6517" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40EF8A0E-8A3C-4BAC-9593-9FF127E8E3D2}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="4800" yWindow="2840" windowWidth="14400" windowHeight="7240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Attendance" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>Employee Name</t>
   </si>
@@ -78,9 +79,6 @@
   </si>
   <si>
     <t>21</t>
-  </si>
-  <si>
-    <t>47.62%</t>
   </si>
   <si>
     <t>Tejaswi</t>
@@ -481,13 +479,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.4140625" customWidth="1"/>
+    <col min="8" max="8" width="11.08203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -538,13 +537,13 @@
       <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
-        <v>15</v>
+      <c r="H2">
+        <v>47.62</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -570,7 +569,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -596,7 +595,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -625,7 +624,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
@@ -648,10 +647,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
         <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
       </c>
       <c r="C7">
         <v>2024</v>
@@ -674,10 +673,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8">
         <v>2024</v>
@@ -700,10 +699,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9">
         <v>2024</v>
@@ -728,7 +727,19 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A2:H2 B1:H1" numberStoredAsText="1"/>
+    <ignoredError sqref="A2:G2 B1:H1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD97F686-3015-49D5-9E2E-3BC8A5814048}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>